<commit_message>
Cleanup of PDS4 code
</commit_message>
<xml_diff>
--- a/observation_lists/CASSINI_OBSERVATION_LIST.xlsx
+++ b/observation_lists/CASSINI_OBSERVATION_LIST.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3857" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3966" uniqueCount="581">
   <si>
     <t xml:space="preserve">Observation</t>
   </si>
@@ -928,7 +928,7 @@
     <t xml:space="preserve">2013-06-01 01:45:33</t>
   </si>
   <si>
-    <t xml:space="preserve">Focuses on five specific co-rotating longitudes for no obvious reason - currently excluded</t>
+    <t xml:space="preserve">Follows one co-rotating longitude</t>
   </si>
   <si>
     <t xml:space="preserve">ISS_191RF_FMOVIE001_PRIME_2</t>
@@ -1111,9 +1111,6 @@
     <t xml:space="preserve">2013-12-06 09:41:49</t>
   </si>
   <si>
-    <t xml:space="preserve">XXX REU: Follows one co-rotating longitude all the way around - currently excluded</t>
-  </si>
-  <si>
     <t xml:space="preserve">ISS_200RI_SPOKEMOV001_PRIME</t>
   </si>
   <si>
@@ -1570,9 +1567,6 @@
     <t xml:space="preserve">2017-01-09 21:10:19</t>
   </si>
   <si>
-    <t xml:space="preserve">Follows one high-resolution co-rotating longitude for about 80 degrees</t>
-  </si>
-  <si>
     <t xml:space="preserve">ISS_260RF_FMOVIE001_PRIME</t>
   </si>
   <si>
@@ -1649,9 +1643,6 @@
   </si>
   <si>
     <t xml:space="preserve">2017-04-03 23:55:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not inertial</t>
   </si>
   <si>
     <t xml:space="preserve">ISS_268RF_FMOVIE001_PRIME_2</t>
@@ -1782,7 +1773,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1803,14 +1794,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1862,7 +1845,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1879,15 +1862,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1911,9 +1890,9 @@
   <dimension ref="A1:T297"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G228" activeCellId="0" sqref="G228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5020,7 +4999,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="s">
+      <c r="A55" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B55" s="2"/>
@@ -5030,6 +5009,9 @@
       <c r="I55" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="J55" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="K55" s="1" t="s">
         <v>21</v>
       </c>
@@ -5049,7 +5031,7 @@
         <v>19</v>
       </c>
       <c r="Q55" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="R55" s="1" t="s">
         <v>19</v>
@@ -5334,7 +5316,7 @@
       <c r="P60" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q60" s="5" t="s">
+      <c r="Q60" s="4" t="s">
         <v>21</v>
       </c>
       <c r="R60" s="1" t="s">
@@ -6692,13 +6674,49 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B85" s="2"/>
+      <c r="H85" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M85" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N85" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O85" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P85" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q85" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R85" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S85" s="0" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="6" t="s">
+      <c r="A86" s="5" t="s">
         <v>189</v>
       </c>
       <c r="B86" s="2" t="s">
@@ -6813,7 +6831,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="3" t="s">
         <v>196</v>
       </c>
       <c r="B88" s="2"/>
@@ -6822,6 +6840,36 @@
       </c>
       <c r="I88" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="J88" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L88" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M88" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N88" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P88" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S88" s="0" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7167,16 +7215,82 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="4" t="s">
+      <c r="A95" s="3" t="s">
         <v>210</v>
       </c>
       <c r="B95" s="2"/>
+      <c r="H95" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L95" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N95" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q95" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R95" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="3" t="s">
         <v>211</v>
       </c>
       <c r="B96" s="2"/>
+      <c r="H96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M96" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N96" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q96" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R96" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
@@ -9631,7 +9745,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="6" t="s">
+      <c r="A140" s="3" t="s">
         <v>300</v>
       </c>
       <c r="B140" s="2" t="s">
@@ -9653,19 +9767,19 @@
         <v>71.29</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>191</v>
+        <v>24</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>191</v>
+        <v>20</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>192</v>
+        <v>21</v>
       </c>
       <c r="L140" s="1" t="s">
-        <v>192</v>
+        <v>21</v>
       </c>
       <c r="M140" s="1" t="s">
         <v>21</v>
@@ -9674,44 +9788,188 @@
         <v>21</v>
       </c>
       <c r="O140" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P140" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q140" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="R140" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="S140" s="0" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="3" t="s">
         <v>303</v>
       </c>
       <c r="B141" s="2"/>
+      <c r="H141" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I141" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J141" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K141" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L141" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N141" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O141" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P141" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q141" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R141" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S141" s="0" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="6" t="s">
+      <c r="A142" s="3" t="s">
         <v>304</v>
       </c>
       <c r="B142" s="2"/>
+      <c r="H142" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I142" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J142" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K142" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L142" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M142" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N142" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O142" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P142" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q142" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R142" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S142" s="0" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="6" t="s">
+      <c r="A143" s="3" t="s">
         <v>305</v>
       </c>
       <c r="B143" s="2"/>
+      <c r="H143" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J143" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K143" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L143" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M143" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N143" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P143" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q143" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R143" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S143" s="0" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="6" t="s">
+      <c r="A144" s="3" t="s">
         <v>306</v>
       </c>
       <c r="B144" s="2"/>
+      <c r="H144" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I144" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J144" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K144" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L144" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M144" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N144" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P144" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q144" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R144" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S144" s="0" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
@@ -11460,7 +11718,7 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="6" t="s">
+      <c r="A175" s="3" t="s">
         <v>361</v>
       </c>
       <c r="B175" s="2" t="s">
@@ -11482,7 +11740,19 @@
         <v>69.42</v>
       </c>
       <c r="H175" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J175" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K175" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L175" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="M175" s="1" t="s">
         <v>21</v>
@@ -11491,10 +11761,10 @@
         <v>21</v>
       </c>
       <c r="O175" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P175" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="Q175" s="1" t="s">
         <v>21</v>
@@ -11503,15 +11773,15 @@
         <v>21</v>
       </c>
       <c r="S175" s="0" t="s">
-        <v>363</v>
+        <v>302</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="B176" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="C176" s="1" t="n">
         <v>100</v>
@@ -11564,10 +11834,10 @@
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B177" s="2" t="s">
         <v>366</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>367</v>
       </c>
       <c r="C177" s="1" t="n">
         <v>100</v>
@@ -11623,10 +11893,10 @@
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C178" s="1" t="n">
         <v>100</v>
@@ -11682,10 +11952,10 @@
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C179" s="1" t="n">
         <v>100</v>
@@ -11741,10 +12011,10 @@
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B180" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="B180" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="C180" s="1" t="n">
         <v>43.56</v>
@@ -11798,10 +12068,10 @@
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B181" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>373</v>
       </c>
       <c r="C181" s="1" t="n">
         <v>100</v>
@@ -11855,10 +12125,10 @@
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B182" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="B182" s="2" t="s">
-        <v>375</v>
       </c>
       <c r="C182" s="1" t="n">
         <v>100</v>
@@ -11914,10 +12184,10 @@
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C183" s="1" t="n">
         <v>100</v>
@@ -11973,10 +12243,10 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B184" s="2" t="s">
         <v>377</v>
-      </c>
-      <c r="B184" s="2" t="s">
-        <v>378</v>
       </c>
       <c r="C184" s="1" t="n">
         <v>5.17</v>
@@ -12032,10 +12302,10 @@
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B185" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>380</v>
       </c>
       <c r="C185" s="1" t="n">
         <v>3.77</v>
@@ -12091,10 +12361,10 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B186" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="B186" s="2" t="s">
-        <v>382</v>
       </c>
       <c r="C186" s="1" t="n">
         <v>51.57</v>
@@ -12150,10 +12420,10 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B187" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="B187" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="C187" s="1" t="n">
         <v>51.71</v>
@@ -12209,10 +12479,10 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B188" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>386</v>
       </c>
       <c r="C188" s="1" t="n">
         <v>90.75</v>
@@ -12265,10 +12535,10 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B189" s="2" t="s">
         <v>387</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>388</v>
       </c>
       <c r="C189" s="1" t="n">
         <v>100</v>
@@ -12324,7 +12594,7 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B190" s="2"/>
       <c r="H190" s="1" t="s">
@@ -12366,10 +12636,10 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B191" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="B191" s="2" t="s">
-        <v>391</v>
       </c>
       <c r="C191" s="1" t="n">
         <v>100</v>
@@ -12422,10 +12692,10 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B192" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>393</v>
       </c>
       <c r="C192" s="1" t="n">
         <v>100</v>
@@ -12478,10 +12748,10 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B193" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>395</v>
       </c>
       <c r="C193" s="1" t="n">
         <v>100</v>
@@ -12534,10 +12804,10 @@
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B194" s="2" t="s">
         <v>396</v>
-      </c>
-      <c r="B194" s="2" t="s">
-        <v>397</v>
       </c>
       <c r="C194" s="1" t="n">
         <v>45.66</v>
@@ -12591,15 +12861,15 @@
         <v>111</v>
       </c>
       <c r="T194" s="0" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B195" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="B195" s="2" t="s">
-        <v>400</v>
       </c>
       <c r="C195" s="1" t="n">
         <v>44.99</v>
@@ -12655,10 +12925,10 @@
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B196" s="2" t="s">
         <v>401</v>
-      </c>
-      <c r="B196" s="2" t="s">
-        <v>402</v>
       </c>
       <c r="C196" s="1" t="n">
         <v>58.63</v>
@@ -12714,10 +12984,10 @@
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B197" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>404</v>
       </c>
       <c r="C197" s="1" t="n">
         <v>58.31</v>
@@ -12773,10 +13043,10 @@
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B198" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="B198" s="2" t="s">
-        <v>406</v>
       </c>
       <c r="C198" s="1" t="n">
         <v>91.06</v>
@@ -12829,10 +13099,10 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B199" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="C199" s="1" t="n">
         <v>4.77</v>
@@ -12852,16 +13122,16 @@
       <c r="H199" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I199" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J199" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K199" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L199" s="5" t="s">
+      <c r="I199" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J199" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K199" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L199" s="4" t="s">
         <v>21</v>
       </c>
       <c r="M199" s="1" t="s">
@@ -12888,10 +13158,10 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B200" s="2" t="s">
         <v>409</v>
-      </c>
-      <c r="B200" s="2" t="s">
-        <v>410</v>
       </c>
       <c r="C200" s="1" t="n">
         <v>3.86</v>
@@ -12944,7 +13214,7 @@
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B201" s="2"/>
       <c r="H201" s="1" t="s">
@@ -12983,10 +13253,10 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B202" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="B202" s="2" t="s">
-        <v>413</v>
       </c>
       <c r="C202" s="1" t="n">
         <v>4</v>
@@ -13039,10 +13309,10 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B203" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="B203" s="2" t="s">
-        <v>415</v>
       </c>
       <c r="C203" s="1" t="n">
         <v>82.21</v>
@@ -13095,10 +13365,10 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B204" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="B204" s="2" t="s">
-        <v>417</v>
       </c>
       <c r="C204" s="1" t="n">
         <v>3.82</v>
@@ -13154,10 +13424,10 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B205" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="B205" s="2" t="s">
-        <v>419</v>
       </c>
       <c r="C205" s="1" t="n">
         <v>86.87</v>
@@ -13210,10 +13480,10 @@
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B206" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="B206" s="2" t="s">
-        <v>421</v>
       </c>
       <c r="C206" s="1" t="n">
         <v>35.27</v>
@@ -13269,10 +13539,10 @@
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="B207" s="2" t="s">
         <v>422</v>
-      </c>
-      <c r="B207" s="2" t="s">
-        <v>423</v>
       </c>
       <c r="C207" s="1" t="n">
         <v>18.3</v>
@@ -13328,10 +13598,10 @@
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B208" s="2" t="s">
         <v>424</v>
-      </c>
-      <c r="B208" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="C208" s="1" t="n">
         <v>51.83</v>
@@ -13387,10 +13657,10 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B209" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>427</v>
       </c>
       <c r="C209" s="1" t="n">
         <v>49.78</v>
@@ -13446,10 +13716,10 @@
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="B210" s="2" t="s">
         <v>428</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>429</v>
       </c>
       <c r="C210" s="1" t="n">
         <v>46.22</v>
@@ -13505,10 +13775,10 @@
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="B211" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>431</v>
       </c>
       <c r="C211" s="1" t="n">
         <v>44.08</v>
@@ -13564,10 +13834,10 @@
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="B212" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="C212" s="1" t="n">
         <v>100</v>
@@ -13620,10 +13890,10 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="B213" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>435</v>
       </c>
       <c r="C213" s="1" t="n">
         <v>100</v>
@@ -13676,10 +13946,10 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B214" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>437</v>
       </c>
       <c r="C214" s="1" t="n">
         <v>21.99</v>
@@ -13732,10 +14002,10 @@
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="B215" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="B215" s="2" t="s">
-        <v>439</v>
       </c>
       <c r="C215" s="1" t="n">
         <v>45.34</v>
@@ -13791,10 +14061,10 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B216" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="B216" s="2" t="s">
-        <v>441</v>
       </c>
       <c r="C216" s="1" t="n">
         <v>44.79</v>
@@ -13850,10 +14120,10 @@
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B217" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="B217" s="2" t="s">
-        <v>443</v>
       </c>
       <c r="C217" s="1" t="n">
         <v>100</v>
@@ -13904,15 +14174,15 @@
         <v>19</v>
       </c>
       <c r="S217" s="0" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B218" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="B218" s="2" t="s">
-        <v>446</v>
       </c>
       <c r="C218" s="1" t="n">
         <v>94.06</v>
@@ -13964,11 +14234,11 @@
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="6" t="s">
+      <c r="A219" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="B219" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="B219" s="2" t="s">
-        <v>448</v>
       </c>
       <c r="C219" s="1" t="n">
         <v>98.08</v>
@@ -14013,15 +14283,15 @@
         <v>19</v>
       </c>
       <c r="S219" s="0" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="B220" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="B220" s="2" t="s">
-        <v>451</v>
       </c>
       <c r="C220" s="1" t="n">
         <v>95.63</v>
@@ -14074,10 +14344,10 @@
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B221" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="B221" s="2" t="s">
-        <v>453</v>
       </c>
       <c r="C221" s="1" t="n">
         <v>2.81</v>
@@ -14130,10 +14400,10 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="B222" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="B222" s="2" t="s">
-        <v>455</v>
       </c>
       <c r="C222" s="1" t="n">
         <v>95.63</v>
@@ -14189,10 +14459,10 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B223" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>457</v>
       </c>
       <c r="C223" s="1" t="n">
         <v>43.74</v>
@@ -14248,10 +14518,10 @@
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B224" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="B224" s="2" t="s">
-        <v>459</v>
       </c>
       <c r="C224" s="1" t="n">
         <v>52.79</v>
@@ -14307,10 +14577,10 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B225" s="2" t="s">
         <v>460</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>461</v>
       </c>
       <c r="C225" s="1" t="n">
         <v>7.97</v>
@@ -14366,10 +14636,10 @@
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B226" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>463</v>
       </c>
       <c r="C226" s="1" t="n">
         <v>9.44</v>
@@ -14423,10 +14693,10 @@
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B227" s="2" t="s">
         <v>464</v>
-      </c>
-      <c r="B227" s="2" t="s">
-        <v>465</v>
       </c>
       <c r="C227" s="1" t="n">
         <v>43.97</v>
@@ -14479,10 +14749,10 @@
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B228" s="2" t="s">
         <v>466</v>
-      </c>
-      <c r="B228" s="2" t="s">
-        <v>467</v>
       </c>
       <c r="C228" s="1" t="n">
         <v>90.07</v>
@@ -14536,10 +14806,10 @@
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B229" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="B229" s="2" t="s">
-        <v>469</v>
       </c>
       <c r="C229" s="1" t="n">
         <v>89.13</v>
@@ -14592,10 +14862,10 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B230" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="B230" s="2" t="s">
-        <v>471</v>
       </c>
       <c r="C230" s="1" t="n">
         <v>51.82</v>
@@ -14651,10 +14921,10 @@
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B231" s="2" t="s">
         <v>472</v>
-      </c>
-      <c r="B231" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="C231" s="1" t="n">
         <v>48.27</v>
@@ -14710,10 +14980,10 @@
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B232" s="2" t="s">
         <v>474</v>
-      </c>
-      <c r="B232" s="2" t="s">
-        <v>475</v>
       </c>
       <c r="C232" s="1" t="n">
         <v>100</v>
@@ -14766,10 +15036,10 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B233" s="2" t="s">
         <v>476</v>
-      </c>
-      <c r="B233" s="2" t="s">
-        <v>477</v>
       </c>
       <c r="C233" s="1" t="n">
         <v>96.65</v>
@@ -14822,10 +15092,10 @@
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B234" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>479</v>
       </c>
       <c r="C234" s="1" t="n">
         <v>29.08</v>
@@ -14878,10 +15148,10 @@
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="B235" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="B235" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="C235" s="1" t="n">
         <v>10</v>
@@ -14934,10 +15204,10 @@
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B236" s="2" t="s">
         <v>482</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>483</v>
       </c>
       <c r="C236" s="1" t="n">
         <v>52.31</v>
@@ -14993,10 +15263,10 @@
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="B237" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="B237" s="2" t="s">
-        <v>485</v>
       </c>
       <c r="C237" s="1" t="n">
         <v>36.28</v>
@@ -15052,10 +15322,10 @@
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="B238" s="2" t="s">
         <v>486</v>
-      </c>
-      <c r="B238" s="2" t="s">
-        <v>487</v>
       </c>
       <c r="C238" s="1" t="n">
         <v>57.26</v>
@@ -15108,10 +15378,10 @@
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B239" s="2" t="s">
         <v>488</v>
-      </c>
-      <c r="B239" s="2" t="s">
-        <v>489</v>
       </c>
       <c r="C239" s="1" t="n">
         <v>100</v>
@@ -15164,10 +15434,10 @@
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B240" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="B240" s="2" t="s">
-        <v>491</v>
       </c>
       <c r="C240" s="1" t="n">
         <v>100</v>
@@ -15220,10 +15490,10 @@
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B241" s="2" t="s">
         <v>492</v>
-      </c>
-      <c r="B241" s="2" t="s">
-        <v>493</v>
       </c>
       <c r="C241" s="1" t="n">
         <v>44.91</v>
@@ -15279,10 +15549,10 @@
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="B242" s="2" t="s">
         <v>494</v>
-      </c>
-      <c r="B242" s="2" t="s">
-        <v>495</v>
       </c>
       <c r="C242" s="1" t="n">
         <v>43.88</v>
@@ -15338,10 +15608,10 @@
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="B243" s="2" t="s">
         <v>496</v>
-      </c>
-      <c r="B243" s="2" t="s">
-        <v>497</v>
       </c>
       <c r="C243" s="1" t="n">
         <v>14.77</v>
@@ -15394,10 +15664,10 @@
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B244" s="2" t="s">
         <v>498</v>
-      </c>
-      <c r="B244" s="2" t="s">
-        <v>499</v>
       </c>
       <c r="C244" s="1" t="n">
         <v>16.47</v>
@@ -15450,10 +15720,10 @@
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B245" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="B245" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="C245" s="1" t="n">
         <v>100</v>
@@ -15506,10 +15776,10 @@
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="B246" s="2" t="s">
         <v>502</v>
-      </c>
-      <c r="B246" s="2" t="s">
-        <v>503</v>
       </c>
       <c r="C246" s="1" t="n">
         <v>2.13</v>
@@ -15562,10 +15832,10 @@
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="B247" s="2" t="s">
         <v>504</v>
-      </c>
-      <c r="B247" s="2" t="s">
-        <v>505</v>
       </c>
       <c r="C247" s="1" t="n">
         <v>100</v>
@@ -15618,10 +15888,10 @@
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="B248" s="2" t="s">
         <v>506</v>
-      </c>
-      <c r="B248" s="2" t="s">
-        <v>507</v>
       </c>
       <c r="C248" s="1" t="n">
         <v>2.3</v>
@@ -15674,10 +15944,10 @@
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="B249" s="2" t="s">
         <v>508</v>
-      </c>
-      <c r="B249" s="2" t="s">
-        <v>509</v>
       </c>
       <c r="C249" s="1" t="n">
         <v>1.32</v>
@@ -15730,10 +16000,10 @@
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="B250" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="B250" s="2" t="s">
-        <v>511</v>
       </c>
       <c r="C250" s="1" t="n">
         <v>52.88</v>
@@ -15789,10 +16059,10 @@
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="B251" s="2" t="s">
         <v>512</v>
-      </c>
-      <c r="B251" s="2" t="s">
-        <v>513</v>
       </c>
       <c r="C251" s="1" t="n">
         <v>52.66</v>
@@ -15848,10 +16118,10 @@
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="B252" s="2" t="s">
         <v>514</v>
-      </c>
-      <c r="B252" s="2" t="s">
-        <v>515</v>
       </c>
       <c r="C252" s="1" t="n">
         <v>1.64</v>
@@ -15902,15 +16172,15 @@
         <v>21</v>
       </c>
       <c r="S252" s="0" t="s">
-        <v>516</v>
+        <v>302</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="3" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C253" s="1" t="n">
         <v>100</v>
@@ -15963,10 +16233,10 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="3" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C254" s="1" t="n">
         <v>1.46</v>
@@ -16019,7 +16289,7 @@
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="B255" s="2"/>
       <c r="H255" s="1" t="s">
@@ -16056,12 +16326,12 @@
         <v>19</v>
       </c>
       <c r="S255" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="3" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B256" s="2"/>
       <c r="H256" s="1" t="s">
@@ -16098,12 +16368,12 @@
         <v>21</v>
       </c>
       <c r="S256" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="3" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="B257" s="2"/>
       <c r="H257" s="1" t="s">
@@ -16140,12 +16410,12 @@
         <v>21</v>
       </c>
       <c r="S257" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="3" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B258" s="2"/>
       <c r="H258" s="1" t="s">
@@ -16182,12 +16452,12 @@
         <v>21</v>
       </c>
       <c r="S258" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="3" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B259" s="2"/>
       <c r="H259" s="1" t="s">
@@ -16224,12 +16494,12 @@
         <v>21</v>
       </c>
       <c r="S259" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="3" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B260" s="2"/>
       <c r="H260" s="1" t="s">
@@ -16266,12 +16536,12 @@
         <v>21</v>
       </c>
       <c r="S260" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="3" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B261" s="2"/>
       <c r="H261" s="1" t="s">
@@ -16308,12 +16578,12 @@
         <v>21</v>
       </c>
       <c r="S261" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="3" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B262" s="2"/>
       <c r="H262" s="1" t="s">
@@ -16350,12 +16620,12 @@
         <v>21</v>
       </c>
       <c r="S262" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="3" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B263" s="2"/>
       <c r="H263" s="1" t="s">
@@ -16392,12 +16662,12 @@
         <v>21</v>
       </c>
       <c r="S263" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="3" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B264" s="2"/>
       <c r="H264" s="1" t="s">
@@ -16434,12 +16704,12 @@
         <v>21</v>
       </c>
       <c r="S264" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="3" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B265" s="2"/>
       <c r="H265" s="1" t="s">
@@ -16476,30 +16746,54 @@
         <v>21</v>
       </c>
       <c r="S265" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="6" t="s">
-        <v>533</v>
+      <c r="A266" s="3" t="s">
+        <v>531</v>
       </c>
       <c r="B266" s="2"/>
       <c r="H266" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="I266" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J266" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K266" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L266" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="M266" s="1" t="s">
         <v>21</v>
       </c>
       <c r="N266" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="O266" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P266" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q266" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R266" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="S266" s="0" t="s">
-        <v>516</v>
+        <v>302</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="3" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B267" s="2"/>
       <c r="H267" s="1" t="s">
@@ -16536,12 +16830,12 @@
         <v>21</v>
       </c>
       <c r="S267" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="3" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B268" s="2"/>
       <c r="H268" s="1" t="s">
@@ -16578,12 +16872,12 @@
         <v>21</v>
       </c>
       <c r="S268" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="3" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="B269" s="2"/>
       <c r="H269" s="1" t="s">
@@ -16620,12 +16914,12 @@
         <v>21</v>
       </c>
       <c r="S269" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="3" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B270" s="2"/>
       <c r="H270" s="1" t="s">
@@ -16662,12 +16956,12 @@
         <v>21</v>
       </c>
       <c r="S270" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="3" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B271" s="2"/>
       <c r="H271" s="1" t="s">
@@ -16704,15 +16998,15 @@
         <v>21</v>
       </c>
       <c r="S271" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="3" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C272" s="1" t="n">
         <v>30.84</v>
@@ -16765,11 +17059,11 @@
       <c r="S272" s="3"/>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="6" t="s">
-        <v>541</v>
+      <c r="A273" s="3" t="s">
+        <v>539</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C273" s="1" t="n">
         <v>2.36</v>
@@ -16787,7 +17081,19 @@
         <v>63.28</v>
       </c>
       <c r="H273" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="I273" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J273" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K273" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L273" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="M273" s="1" t="s">
         <v>21</v>
@@ -16799,24 +17105,24 @@
         <v>19</v>
       </c>
       <c r="P273" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q273" s="1" t="s">
-        <v>192</v>
+        <v>21</v>
       </c>
       <c r="R273" s="1" t="s">
-        <v>192</v>
+        <v>21</v>
       </c>
       <c r="S273" s="0" t="s">
-        <v>543</v>
+        <v>302</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C274" s="1" t="n">
         <v>3.28</v>
@@ -16867,15 +17173,15 @@
         <v>19</v>
       </c>
       <c r="S274" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="3" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C275" s="1" t="n">
         <v>2.18</v>
@@ -16926,16 +17232,16 @@
         <v>19</v>
       </c>
       <c r="S275" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="3" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B276" s="2"/>
-      <c r="C276" s="5"/>
-      <c r="D276" s="5"/>
+      <c r="C276" s="4"/>
+      <c r="D276" s="4"/>
       <c r="H276" s="1" t="s">
         <v>19</v>
       </c>
@@ -16970,12 +17276,12 @@
         <v>19</v>
       </c>
       <c r="S276" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="3" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B277" s="2"/>
       <c r="H277" s="1" t="s">
@@ -17012,12 +17318,12 @@
         <v>19</v>
       </c>
       <c r="S277" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="3" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B278" s="2"/>
       <c r="H278" s="1" t="s">
@@ -17054,12 +17360,12 @@
         <v>19</v>
       </c>
       <c r="S278" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="3" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="B279" s="2"/>
       <c r="H279" s="1" t="s">
@@ -17096,12 +17402,12 @@
         <v>19</v>
       </c>
       <c r="S279" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="3" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B280" s="2"/>
       <c r="H280" s="1" t="s">
@@ -17138,12 +17444,12 @@
         <v>19</v>
       </c>
       <c r="S280" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="3" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B281" s="2"/>
       <c r="H281" s="1" t="s">
@@ -17180,15 +17486,15 @@
         <v>19</v>
       </c>
       <c r="S281" s="0" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="3" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C282" s="1" t="n">
         <v>55.07</v>
@@ -17241,10 +17547,10 @@
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="3" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C283" s="1" t="n">
         <v>37.04</v>
@@ -17297,10 +17603,10 @@
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="3" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C284" s="1" t="n">
         <v>78.72</v>
@@ -17353,10 +17659,10 @@
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="3" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C285" s="1" t="n">
         <v>91.78</v>
@@ -17409,7 +17715,7 @@
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="3" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B286" s="2"/>
       <c r="H286" s="1" t="s">
@@ -17451,7 +17757,7 @@
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="3" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B287" s="2"/>
       <c r="H287" s="1" t="s">
@@ -17493,10 +17799,10 @@
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="3" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C288" s="1" t="n">
         <v>13.14</v>
@@ -17549,10 +17855,10 @@
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="3" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C289" s="1" t="n">
         <v>34.62</v>
@@ -17605,10 +17911,10 @@
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C290" s="1" t="n">
         <v>5.93</v>
@@ -17661,10 +17967,10 @@
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="3" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C291" s="1" t="n">
         <v>3.89</v>
@@ -17717,10 +18023,10 @@
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="3" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="C292" s="1" t="n">
         <v>4.7</v>
@@ -17771,15 +18077,15 @@
         <v>19</v>
       </c>
       <c r="S292" s="0" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C293" s="1" t="n">
         <v>3.68</v>
@@ -17832,10 +18138,10 @@
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="3" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C294" s="1" t="n">
         <v>100</v>
@@ -17888,10 +18194,10 @@
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="3" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C295" s="1" t="n">
         <v>100</v>
@@ -17944,10 +18250,10 @@
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="3" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C296" s="1" t="n">
         <v>2.83</v>
@@ -18000,10 +18306,10 @@
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="3" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C297" s="1" t="n">
         <v>5.31</v>

</xml_diff>